<commit_message>
added method to input array of light positions and test ui elements
</commit_message>
<xml_diff>
--- a/other/Project_TimeLine_2021_8_Apr.xlsx
+++ b/other/Project_TimeLine_2021_8_Apr.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Murphy Tan\Desktop\aztech-lms\other\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6AAA494-3B89-4816-A2E6-6AF8ACDE0AB5}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{637BFEA0-66FD-400B-A052-265B4A605DDB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13140" xr2:uid="{5A8E5395-CCD6-4F57-83A8-81B53FE4AFF6}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="36">
   <si>
     <t>S/N</t>
   </si>
@@ -141,11 +141,7 @@
     <t>Front-end: Dashboard view data management</t>
   </si>
   <si>
-    <t>By moving data out of the individual card components, potentially less API calls will be required</t>
-  </si>
-  <si>
-    <t>Work on this at least till new pages or content added to Adobe XD link
-Expected to take a long time as it was originally not written in React, and I foresee some issues arising from that</t>
+    <t>To split into smaller tasks</t>
   </si>
 </sst>
 </file>
@@ -529,7 +525,7 @@
   <dimension ref="A1:I28"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H21" sqref="H21"/>
+      <selection activeCell="H25" sqref="H25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -993,7 +989,7 @@
       </c>
       <c r="H19" s="4"/>
     </row>
-    <row r="20" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>19</v>
       </c>
@@ -1015,11 +1011,9 @@
       <c r="G20" s="3">
         <v>44287</v>
       </c>
-      <c r="I20" s="4" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" ht="120" x14ac:dyDescent="0.25">
+      <c r="I20" s="4"/>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>20</v>
       </c>
@@ -1038,10 +1032,10 @@
       <c r="F21" s="3">
         <v>44300</v>
       </c>
-      <c r="H21" s="4"/>
-      <c r="I21" s="4" t="s">
-        <v>36</v>
-      </c>
+      <c r="H21" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="I21" s="4"/>
     </row>
     <row r="26" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="B26" t="s">

</xml_diff>